<commit_message>
changed gerbers and price list
</commit_message>
<xml_diff>
--- a/Price List/Roboter Arm Main Controller.xlsx
+++ b/Price List/Roboter Arm Main Controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TH24\Desktop\Hardware\Robotic-Arm\Price List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65614FC3-5A7D-4E56-AF90-F8F6261AD16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB736525-F68C-4D9C-A9B1-EB94639F7DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="945" windowWidth="26025" windowHeight="14535" xr2:uid="{6B6AC393-9DA6-4B7B-AC95-3B83A5A5BB6E}"/>
   </bookViews>
@@ -984,13 +984,13 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" customWidth="1"/>
     <col min="3" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
   </cols>

</xml_diff>